<commit_message>
Dlya loha bez excel
</commit_message>
<xml_diff>
--- a/python/Upwork.xlsx
+++ b/python/Upwork.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OscarOyomba\OneDrive - pesapal.com\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corol\Desktop\Home\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="21570" windowHeight="10215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>Company</t>
   </si>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,7 +80,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -94,9 +96,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -134,7 +136,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -206,7 +208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -356,43 +358,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:C7"/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="B2">
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="B3">
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="B4">
         <v>600</v>
       </c>
     </row>

</xml_diff>